<commit_message>
Prepared for LongGold Server use, added Burlington House, added some TPT fix data code
</commit_message>
<xml_diff>
--- a/data/school_def.xlsx
+++ b/data/school_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\analysis\longgold-data-compilation\compile-data\dat_2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\shiny_apps\longgold_monitor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB1EFDE-A0F1-40E1-9595-BC7F7F7AD094}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446C4FDB-D6FB-4134-B528-710789ADF051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
   </bookViews>
   <sheets>
     <sheet name="Years_SchoolsParticipating" sheetId="1" r:id="rId1"/>
@@ -22,17 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="147">
   <si>
     <t>test_year</t>
   </si>
@@ -467,6 +462,12 @@
   </si>
   <si>
     <t>academic_selection</t>
+  </si>
+  <si>
+    <t>BHS</t>
+  </si>
+  <si>
+    <t>Burlington House School</t>
   </si>
 </sst>
 </file>
@@ -843,7 +844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA13A75-6981-BA45-8D0C-D92562E446DD}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D54"/>
     </sheetView>
   </sheetViews>
@@ -2112,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82BB11C-73CE-C64B-825A-E13C90EF0B0E}">
   <dimension ref="A1:AR106"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
@@ -4611,10 +4612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27449B8-1B27-E048-B484-106C08767B7E}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4747,19 +4748,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
         <v>46</v>
@@ -4767,16 +4768,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
@@ -4787,16 +4788,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
@@ -4807,36 +4808,36 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
         <v>48</v>
@@ -4847,61 +4848,81 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small fixes, update school_def for Litvian schools
</commit_message>
<xml_diff>
--- a/data/school_def.xlsx
+++ b/data/school_def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\shiny_apps\longgold_monitor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446C4FDB-D6FB-4134-B528-710789ADF051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D7026-6C77-4CD4-96E3-41307B541B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
   </bookViews>
   <sheets>
     <sheet name="Years_SchoolsParticipating" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="154">
   <si>
     <t>test_year</t>
   </si>
@@ -468,6 +468,27 @@
   </si>
   <si>
     <t>Burlington House School</t>
+  </si>
+  <si>
+    <t>EDM</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>Emils Darzins Music School</t>
+  </si>
+  <si>
+    <t>RCC</t>
+  </si>
+  <si>
+    <t>Riga Cathedral Choir School </t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>Riga Secondary School No 49</t>
   </si>
 </sst>
 </file>
@@ -844,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA13A75-6981-BA45-8D0C-D92562E446DD}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D54"/>
     </sheetView>
   </sheetViews>
@@ -4612,10 +4633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27449B8-1B27-E048-B484-106C08767B7E}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4926,6 +4947,57 @@
         <v>46</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added school 04 REG for LV
</commit_message>
<xml_diff>
--- a/data/school_def.xlsx
+++ b/data/school_def.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\shiny_apps\longgold_monitor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2D7026-6C77-4CD4-96E3-41307B541B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F34767F-F930-4FD5-86CA-35F6AA441B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Test_Batteries" sheetId="3" r:id="rId2"/>
     <sheet name="school_info" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="155">
   <si>
     <t>test_year</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>Riga Secondary School No 49</t>
+  </si>
+  <si>
+    <t>REG</t>
   </si>
 </sst>
 </file>
@@ -4633,10 +4636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27449B8-1B27-E048-B484-106C08767B7E}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4998,6 +5001,23 @@
         <v>48</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added school 05 BCH for LV
</commit_message>
<xml_diff>
--- a/data/school_def.xlsx
+++ b/data/school_def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\shiny_apps\longgold_monitor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F34767F-F930-4FD5-86CA-35F6AA441B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADEE4E0-C91D-47FB-8DE6-DA8506E58E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E493F727-79CA-F141-87BF-2392C9ADD446}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="157">
   <si>
     <t>test_year</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>REG</t>
+  </si>
+  <si>
+    <t>BCH</t>
+  </si>
+  <si>
+    <t>Boys choir (Reinis)</t>
   </si>
 </sst>
 </file>
@@ -4636,10 +4642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27449B8-1B27-E048-B484-106C08767B7E}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5018,6 +5024,20 @@
         <v>48</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>